<commit_message>
Rmarkdown report for catalogueR results
</commit_message>
<xml_diff>
--- a/data/GCST90000255and6_GRCh38_Plessthan1eMinus5_combined_pruned.xlsx
+++ b/data/GCST90000255and6_GRCh38_Plessthan1eMinus5_combined_pruned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ChangMoon/Desktop/Academe/Research/Sinai 2019-2020 Research Projects/Huang Lab/PheWAS/Figures/Supplementary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schilder/Library/Containers/com.microsoft.Excel/Data/Desktop/COVID19_GWAS/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FDF389-BD21-BA48-84D5-276FBC4F5077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A347ABD-1005-6140-B445-7A3F081F5B02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="266 pruned (2)" sheetId="4" r:id="rId1"/>
@@ -1380,15 +1380,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E2E67A-C4F0-774C-94D3-FE6F86977D07}">
-  <dimension ref="A1:P50"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>62</v>
       </c>
@@ -1419,16 +1419,14 @@
       <c r="J1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="15"/>
+      <c r="K1" s="15" t="s">
+        <v>144</v>
+      </c>
       <c r="L1" s="15"/>
-      <c r="M1" s="15" t="s">
-        <v>144</v>
-      </c>
+      <c r="M1" s="15"/>
       <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>64</v>
       </c>
@@ -1459,16 +1457,14 @@
       <c r="J2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="15"/>
+      <c r="K2" s="20" t="s">
+        <v>122</v>
+      </c>
       <c r="L2" s="15"/>
-      <c r="M2" s="20" t="s">
-        <v>122</v>
-      </c>
+      <c r="M2" s="15"/>
       <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>63</v>
       </c>
@@ -1499,16 +1495,14 @@
       <c r="J3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="15"/>
+      <c r="K3" s="20" t="s">
+        <v>123</v>
+      </c>
       <c r="L3" s="15"/>
-      <c r="M3" s="20" t="s">
-        <v>123</v>
-      </c>
+      <c r="M3" s="15"/>
       <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>65</v>
       </c>
@@ -1539,16 +1533,14 @@
       <c r="J4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="15"/>
+      <c r="K4" s="20" t="s">
+        <v>124</v>
+      </c>
       <c r="L4" s="15"/>
-      <c r="M4" s="20" t="s">
-        <v>124</v>
-      </c>
+      <c r="M4" s="15"/>
       <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>67</v>
       </c>
@@ -1579,16 +1571,14 @@
       <c r="J5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="15"/>
+      <c r="K5" s="20" t="s">
+        <v>125</v>
+      </c>
       <c r="L5" s="15"/>
-      <c r="M5" s="20" t="s">
-        <v>125</v>
-      </c>
+      <c r="M5" s="15"/>
       <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>68</v>
       </c>
@@ -1619,16 +1609,14 @@
       <c r="J6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="15"/>
+      <c r="K6" s="20" t="s">
+        <v>126</v>
+      </c>
       <c r="L6" s="15"/>
-      <c r="M6" s="20" t="s">
-        <v>126</v>
-      </c>
+      <c r="M6" s="15"/>
       <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>71</v>
       </c>
@@ -1659,16 +1647,14 @@
       <c r="J7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="15"/>
+      <c r="K7" s="20" t="s">
+        <v>127</v>
+      </c>
       <c r="L7" s="15"/>
-      <c r="M7" s="20" t="s">
-        <v>127</v>
-      </c>
+      <c r="M7" s="15"/>
       <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>79</v>
       </c>
@@ -1699,16 +1685,14 @@
       <c r="J8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K8" s="15"/>
+      <c r="K8" s="20" t="s">
+        <v>128</v>
+      </c>
       <c r="L8" s="15"/>
-      <c r="M8" s="20" t="s">
-        <v>128</v>
-      </c>
+      <c r="M8" s="15"/>
       <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>80</v>
       </c>
@@ -1739,16 +1723,14 @@
       <c r="J9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K9" s="15"/>
+      <c r="K9" s="20" t="s">
+        <v>129</v>
+      </c>
       <c r="L9" s="15"/>
-      <c r="M9" s="20" t="s">
-        <v>129</v>
-      </c>
+      <c r="M9" s="15"/>
       <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>82</v>
       </c>
@@ -1779,16 +1761,14 @@
       <c r="J10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="15"/>
+      <c r="K10" s="20" t="s">
+        <v>130</v>
+      </c>
       <c r="L10" s="15"/>
-      <c r="M10" s="20" t="s">
-        <v>130</v>
-      </c>
+      <c r="M10" s="15"/>
       <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>120</v>
       </c>
@@ -1819,16 +1799,14 @@
       <c r="J11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="15"/>
+      <c r="K11" s="20" t="s">
+        <v>131</v>
+      </c>
       <c r="L11" s="15"/>
-      <c r="M11" s="20" t="s">
-        <v>131</v>
-      </c>
+      <c r="M11" s="15"/>
       <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>85</v>
       </c>
@@ -1859,16 +1837,14 @@
       <c r="J12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="15"/>
+      <c r="K12" s="20" t="s">
+        <v>132</v>
+      </c>
       <c r="L12" s="15"/>
-      <c r="M12" s="20" t="s">
-        <v>132</v>
-      </c>
+      <c r="M12" s="15"/>
       <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>83</v>
       </c>
@@ -1899,16 +1875,14 @@
       <c r="J13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="15"/>
+      <c r="K13" s="20" t="s">
+        <v>133</v>
+      </c>
       <c r="L13" s="15"/>
-      <c r="M13" s="20" t="s">
-        <v>133</v>
-      </c>
+      <c r="M13" s="15"/>
       <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
         <v>87</v>
       </c>
@@ -1939,16 +1913,14 @@
       <c r="J14" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="15"/>
+      <c r="K14" s="20" t="s">
+        <v>134</v>
+      </c>
       <c r="L14" s="15"/>
-      <c r="M14" s="20" t="s">
-        <v>134</v>
-      </c>
+      <c r="M14" s="15"/>
       <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>88</v>
       </c>
@@ -1979,16 +1951,14 @@
       <c r="J15" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="15"/>
+      <c r="K15" s="20" t="s">
+        <v>135</v>
+      </c>
       <c r="L15" s="15"/>
-      <c r="M15" s="20" t="s">
-        <v>135</v>
-      </c>
+      <c r="M15" s="15"/>
       <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>90</v>
       </c>
@@ -2019,16 +1989,14 @@
       <c r="J16" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="15"/>
+      <c r="K16" s="20" t="s">
+        <v>136</v>
+      </c>
       <c r="L16" s="15"/>
-      <c r="M16" s="20" t="s">
-        <v>136</v>
-      </c>
+      <c r="M16" s="15"/>
       <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>91</v>
       </c>
@@ -2059,16 +2027,14 @@
       <c r="J17" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="15"/>
+      <c r="K17" s="20" t="s">
+        <v>137</v>
+      </c>
       <c r="L17" s="15"/>
-      <c r="M17" s="20" t="s">
-        <v>137</v>
-      </c>
+      <c r="M17" s="15"/>
       <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>95</v>
       </c>
@@ -2099,16 +2065,14 @@
       <c r="J18" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K18" s="15"/>
+      <c r="K18" s="20" t="s">
+        <v>138</v>
+      </c>
       <c r="L18" s="15"/>
-      <c r="M18" s="20" t="s">
-        <v>138</v>
-      </c>
+      <c r="M18" s="15"/>
       <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
         <v>98</v>
       </c>
@@ -2139,16 +2103,14 @@
       <c r="J19" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="15"/>
+      <c r="K19" s="20" t="s">
+        <v>139</v>
+      </c>
       <c r="L19" s="15"/>
-      <c r="M19" s="20" t="s">
-        <v>139</v>
-      </c>
+      <c r="M19" s="15"/>
       <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
         <v>100</v>
       </c>
@@ -2179,16 +2141,14 @@
       <c r="J20" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K20" s="15"/>
+      <c r="K20" s="20" t="s">
+        <v>140</v>
+      </c>
       <c r="L20" s="15"/>
-      <c r="M20" s="20" t="s">
-        <v>140</v>
-      </c>
+      <c r="M20" s="15"/>
       <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
         <v>103</v>
       </c>
@@ -2219,16 +2179,14 @@
       <c r="J21" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K21" s="15"/>
+      <c r="K21" s="20" t="s">
+        <v>141</v>
+      </c>
       <c r="L21" s="15"/>
-      <c r="M21" s="20" t="s">
-        <v>141</v>
-      </c>
+      <c r="M21" s="15"/>
       <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
         <v>101</v>
       </c>
@@ -2259,16 +2217,14 @@
       <c r="J22" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K22" s="15"/>
+      <c r="K22" s="20" t="s">
+        <v>142</v>
+      </c>
       <c r="L22" s="15"/>
-      <c r="M22" s="20" t="s">
-        <v>142</v>
-      </c>
+      <c r="M22" s="15"/>
       <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
         <v>102</v>
       </c>
@@ -2299,16 +2255,14 @@
       <c r="J23" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K23" s="15"/>
+      <c r="K23" s="20" t="s">
+        <v>143</v>
+      </c>
       <c r="L23" s="15"/>
-      <c r="M23" s="20" t="s">
-        <v>143</v>
-      </c>
+      <c r="M23" s="15"/>
       <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -2323,10 +2277,8 @@
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
       <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -2340,10 +2292,8 @@
       <c r="K25" s="15"/>
       <c r="L25" s="15"/>
       <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -2357,10 +2307,8 @@
       <c r="K26" s="15"/>
       <c r="L26" s="15"/>
       <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -2374,10 +2322,8 @@
       <c r="K27" s="15"/>
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -2391,10 +2337,8 @@
       <c r="K28" s="15"/>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -2408,10 +2352,8 @@
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
       <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -2425,10 +2367,8 @@
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -2442,10 +2382,8 @@
       <c r="K31" s="15"/>
       <c r="L31" s="15"/>
       <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -2459,10 +2397,8 @@
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -2476,10 +2412,8 @@
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
       <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -2493,10 +2427,8 @@
       <c r="K34" s="15"/>
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -2510,10 +2442,8 @@
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="15"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -2527,10 +2457,8 @@
       <c r="K36" s="15"/>
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -2544,10 +2472,8 @@
       <c r="K37" s="15"/>
       <c r="L37" s="15"/>
       <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="15"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -2561,10 +2487,8 @@
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -2578,10 +2502,8 @@
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -2595,10 +2517,8 @@
       <c r="K40" s="15"/>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -2612,10 +2532,8 @@
       <c r="K41" s="15"/>
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -2629,10 +2547,8 @@
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -2646,10 +2562,8 @@
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="15"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
@@ -2663,10 +2577,8 @@
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="15"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -2680,10 +2592,8 @@
       <c r="K45" s="15"/>
       <c r="L45" s="15"/>
       <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -2697,10 +2607,8 @@
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -2714,10 +2622,8 @@
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="15"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -2731,10 +2637,8 @@
       <c r="K48" s="15"/>
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="15"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -2748,10 +2652,8 @@
       <c r="K49" s="15"/>
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
-      <c r="N49" s="15"/>
-      <c r="O49" s="15"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
@@ -2765,8 +2667,6 @@
       <c r="K50" s="15"/>
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
-      <c r="N50" s="15"/>
-      <c r="O50" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J23" xr:uid="{88B14128-2585-E944-BEA7-0655F3278933}">

</xml_diff>